<commit_message>
Added 7 CATID/Company Name Negative Search Test Cases
</commit_message>
<xml_diff>
--- a/Data Files/Search_CAT_ID_Data - Neg.xlsx
+++ b/Data Files/Search_CAT_ID_Data - Neg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\git\src\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9889FD4-802F-45F9-8A30-63E1AAB4DC45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C7EDF3-472C-400F-BFAE-085A08C31E48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{56648964-8086-4401-B8BD-AFCFF037A6DE}"/>
+    <workbookView xWindow="25065" yWindow="2070" windowWidth="28800" windowHeight="10905" xr2:uid="{56648964-8086-4401-B8BD-AFCFF037A6DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,45 +31,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Gosport</t>
-  </si>
-  <si>
-    <t>Orkney</t>
-  </si>
-  <si>
-    <t>Rugby</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>tradeName</t>
   </si>
   <si>
-    <t>Gosport, Hampshire</t>
-  </si>
-  <si>
-    <t>Banbury, Oxfordshire</t>
-  </si>
-  <si>
-    <t>Selsey</t>
-  </si>
-  <si>
-    <t>Bognor Regis</t>
-  </si>
-  <si>
-    <t>tradeNameLocation</t>
-  </si>
-  <si>
-    <t>tradeNameLocationVerification</t>
-  </si>
-  <si>
-    <t>Retford, Nottinghamshire</t>
-  </si>
-  <si>
-    <t>Rustington</t>
-  </si>
-  <si>
-    <t>Rustington, West Sussex</t>
+    <t>Glazing Solubtions</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>typo</t>
+  </si>
+  <si>
+    <t>above company extra digi</t>
+  </si>
+  <si>
+    <t>z1</t>
+  </si>
+  <si>
+    <t>combi of char and dig</t>
+  </si>
+  <si>
+    <t>6 zeros</t>
+  </si>
+  <si>
+    <t>000000</t>
+  </si>
+  <si>
+    <t>oooooo</t>
+  </si>
+  <si>
+    <t>6 lower case o</t>
+  </si>
+  <si>
+    <t>OOOOOO</t>
+  </si>
+  <si>
+    <t>6 Upper case O</t>
+  </si>
+  <si>
+    <t>1111111111111111111111111111111111111111111111111111111111111111111111111111111111111111111111</t>
+  </si>
+  <si>
+    <t>Number 1s</t>
+  </si>
+  <si>
+    <t>Special Chars</t>
+  </si>
+  <si>
+    <t>£!_+@~#?|*</t>
   </si>
 </sst>
 </file>
@@ -111,12 +123,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D56B88-33E9-468B-853E-05EE5D8A6600}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,68 +467,75 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>3811989</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>218020</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>402921</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>308682</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>230761</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>381198</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CAT search test tweeks for neg testing
</commit_message>
<xml_diff>
--- a/Data Files/Search_CAT_ID_Data - Neg.xlsx
+++ b/Data Files/Search_CAT_ID_Data - Neg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\git\src\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C7EDF3-472C-400F-BFAE-085A08C31E48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E152C8EB-577E-4F86-84DA-266A8F8DE33D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25065" yWindow="2070" windowWidth="28800" windowHeight="10905" xr2:uid="{56648964-8086-4401-B8BD-AFCFF037A6DE}"/>
+    <workbookView xWindow="1110" yWindow="2730" windowWidth="28800" windowHeight="10905" xr2:uid="{56648964-8086-4401-B8BD-AFCFF037A6DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>tradeName</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>£!_+@~#?|*</t>
+  </si>
+  <si>
+    <t>3811989</t>
   </si>
 </sst>
 </file>
@@ -450,7 +453,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A10" sqref="A10:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,8 +485,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>3811989</v>
+      <c r="A3" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>4</v>

</xml_diff>